<commit_message>
working on task gen
</commit_message>
<xml_diff>
--- a/tests/videos/horizon/task-meta.xlsx
+++ b/tests/videos/horizon/task-meta.xlsx
@@ -606,7 +606,7 @@
       </c>
       <c r="AJ1" s="1" t="inlineStr">
         <is>
-          <t>debug</t>
+          <t>is_debug</t>
         </is>
       </c>
       <c r="AK1" s="1" t="inlineStr">
@@ -781,7 +781,7 @@
       </c>
       <c r="AO2" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C</t>
         </is>
       </c>
       <c r="AP2" t="inlineStr">

</xml_diff>